<commit_message>
First complete version inspire
</commit_message>
<xml_diff>
--- a/inspire/GEO-DCAT-AP-Profile.xlsx
+++ b/inspire/GEO-DCAT-AP-Profile.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2674" uniqueCount="1048">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2674" uniqueCount="1050">
   <si>
     <t>uri schema</t>
   </si>
@@ -3174,6 +3174,12 @@
   </si>
   <si>
     <t>This field is required when the temporal reference system is not Gregorian (the common default)</t>
+  </si>
+  <si>
+    <t>ResponsiblePartyRole</t>
+  </si>
+  <si>
+    <t>ResponsibleParty</t>
   </si>
 </sst>
 </file>
@@ -6141,8 +6147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6234,7 +6240,7 @@
         <v>41</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>287</v>
@@ -6275,7 +6281,7 @@
         <v>41</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>287</v>
@@ -6314,7 +6320,7 @@
         <v>41</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>287</v>
@@ -6905,7 +6911,7 @@
         <v>115</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="K19" t="s">
         <v>502</v>
@@ -7146,7 +7152,7 @@
         <v>196</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L25" s="4" t="s">
         <v>290</v>
@@ -7187,7 +7193,7 @@
         <v>198</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L26" s="4" t="s">
         <v>289</v>
@@ -7266,7 +7272,7 @@
         <v>97</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K28" t="s">
         <v>749</v>
@@ -7387,7 +7393,7 @@
         <v>41</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L31" s="4" t="s">
         <v>289</v>
@@ -7580,7 +7586,7 @@
         <v>110</v>
       </c>
       <c r="J36" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K36" t="s">
         <v>310</v>
@@ -7621,7 +7627,7 @@
         <v>102</v>
       </c>
       <c r="J37" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L37" s="4" t="s">
         <v>289</v>
@@ -7697,7 +7703,7 @@
         <v>110</v>
       </c>
       <c r="J39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K39" t="s">
         <v>111</v>
@@ -7929,7 +7935,7 @@
         <v>47</v>
       </c>
       <c r="J45" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K45" t="s">
         <v>312</v>
@@ -7967,7 +7973,7 @@
         <v>46</v>
       </c>
       <c r="J46" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L46" t="s">
         <v>290</v>
@@ -8046,7 +8052,7 @@
         <v>41</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L48" s="4" t="s">
         <v>290</v>
@@ -9342,7 +9348,7 @@
         <v>287</v>
       </c>
       <c r="M84" t="s">
-        <v>511</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
@@ -9377,7 +9383,7 @@
         <v>287</v>
       </c>
       <c r="M85" t="s">
-        <v>511</v>
+        <v>1049</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Found solution for multiple codelists
</commit_message>
<xml_diff>
--- a/inspire/GEO-DCAT-AP-Profile.xlsx
+++ b/inspire/GEO-DCAT-AP-Profile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="7485" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="7485" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="URI schema" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2674" uniqueCount="1050">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2712" uniqueCount="1050">
   <si>
     <t>uri schema</t>
   </si>
@@ -2043,9 +2043,6 @@
     <t>Place-Continent</t>
   </si>
   <si>
-    <t>Place-Contry</t>
-  </si>
-  <si>
     <t>Place-Place</t>
   </si>
   <si>
@@ -2074,12 +2071,6 @@
   </si>
   <si>
     <t>IANA-Application</t>
-  </si>
-  <si>
-    <t>IANA application mediatypes</t>
-  </si>
-  <si>
-    <t>http://www.iana.org/assignments/media-types</t>
   </si>
   <si>
     <t>Total list is larger, Inspire only has three</t>
@@ -3180,6 +3171,15 @@
   </si>
   <si>
     <t>ResponsibleParty</t>
+  </si>
+  <si>
+    <t>http://inspire.ec.europa.eu/theme{waarde}</t>
+  </si>
+  <si>
+    <t>http://inspire.ec.europa.eu/metadata-codelist/ResponsiblePartyRole/{waarde}</t>
+  </si>
+  <si>
+    <t>http://www.geonames.org</t>
   </si>
 </sst>
 </file>
@@ -3591,10 +3591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3628,7 +3628,7 @@
         <v>48</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3748,10 +3748,10 @@
         <v>263</v>
       </c>
       <c r="D10" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="G10" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -3765,10 +3765,10 @@
         <v>263</v>
       </c>
       <c r="D11" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="G11" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3782,7 +3782,7 @@
         <v>263</v>
       </c>
       <c r="D12" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="G12" t="s">
         <v>304</v>
@@ -3799,7 +3799,7 @@
         <v>263</v>
       </c>
       <c r="D13" t="s">
-        <v>516</v>
+        <v>1047</v>
       </c>
       <c r="G13" t="s">
         <v>306</v>
@@ -3816,7 +3816,7 @@
         <v>263</v>
       </c>
       <c r="D14" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="G14" t="s">
         <v>104</v>
@@ -3833,7 +3833,7 @@
         <v>263</v>
       </c>
       <c r="D15" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="G15" t="s">
         <v>310</v>
@@ -3850,7 +3850,7 @@
         <v>263</v>
       </c>
       <c r="D16" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="G16" t="s">
         <v>312</v>
@@ -3867,7 +3867,7 @@
         <v>263</v>
       </c>
       <c r="D17" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="G17" t="s">
         <v>670</v>
@@ -3884,10 +3884,10 @@
         <v>263</v>
       </c>
       <c r="D18" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="G18" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -3901,10 +3901,10 @@
         <v>263</v>
       </c>
       <c r="D19" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="G19" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -3918,7 +3918,7 @@
         <v>263</v>
       </c>
       <c r="D20" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="G20" t="s">
         <v>324</v>
@@ -3935,7 +3935,7 @@
         <v>263</v>
       </c>
       <c r="D21" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="G21" t="s">
         <v>325</v>
@@ -3952,7 +3952,7 @@
         <v>263</v>
       </c>
       <c r="D22" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="G22" t="s">
         <v>299</v>
@@ -3969,7 +3969,7 @@
         <v>263</v>
       </c>
       <c r="D23" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="G23" t="s">
         <v>502</v>
@@ -3986,10 +3986,10 @@
         <v>263</v>
       </c>
       <c r="D24" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="G24" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -4003,10 +4003,10 @@
         <v>263</v>
       </c>
       <c r="D25" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="G25" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -4020,10 +4020,10 @@
         <v>263</v>
       </c>
       <c r="D26" t="s">
-        <v>1027</v>
+        <v>1024</v>
       </c>
       <c r="G26" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -4031,13 +4031,16 @@
         <v>262</v>
       </c>
       <c r="B27" t="s">
-        <v>260</v>
+        <v>261</v>
+      </c>
+      <c r="C27" t="s">
+        <v>263</v>
       </c>
       <c r="D27" t="s">
-        <v>703</v>
+        <v>1048</v>
       </c>
       <c r="G27" t="s">
-        <v>299</v>
+        <v>863</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -4048,10 +4051,10 @@
         <v>260</v>
       </c>
       <c r="D28" t="s">
-        <v>705</v>
+        <v>901</v>
       </c>
       <c r="G28" t="s">
-        <v>706</v>
+        <v>863</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -4062,10 +4065,10 @@
         <v>260</v>
       </c>
       <c r="D29" t="s">
-        <v>751</v>
+        <v>700</v>
       </c>
       <c r="G29" t="s">
-        <v>749</v>
+        <v>299</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -4076,245 +4079,245 @@
         <v>260</v>
       </c>
       <c r="D30" t="s">
-        <v>1025</v>
+        <v>702</v>
       </c>
       <c r="G30" t="s">
-        <v>1019</v>
+        <v>703</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>262</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>260</v>
       </c>
       <c r="D31" t="s">
-        <v>13</v>
-      </c>
-      <c r="E31" t="s">
-        <v>2</v>
+        <v>748</v>
+      </c>
+      <c r="G31" t="s">
+        <v>746</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>262</v>
+      </c>
+      <c r="B32" t="s">
+        <v>260</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1022</v>
+      </c>
+      <c r="G32" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>262</v>
+      </c>
+      <c r="B33" t="s">
+        <v>260</v>
+      </c>
+      <c r="D33" t="s">
+        <v>677</v>
+      </c>
+      <c r="G33" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>262</v>
+      </c>
+      <c r="B34" t="s">
+        <v>260</v>
+      </c>
+      <c r="D34" t="s">
+        <v>677</v>
+      </c>
+      <c r="G34" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>262</v>
+      </c>
+      <c r="B35" t="s">
+        <v>260</v>
+      </c>
+      <c r="D35" t="s">
+        <v>373</v>
+      </c>
+      <c r="G35" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>262</v>
+      </c>
+      <c r="B36" t="s">
+        <v>260</v>
+      </c>
+      <c r="D36" t="s">
+        <v>319</v>
+      </c>
+      <c r="G36" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>262</v>
+      </c>
+      <c r="B37" t="s">
+        <v>260</v>
+      </c>
+      <c r="D37" t="s">
+        <v>317</v>
+      </c>
+      <c r="G37" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>262</v>
+      </c>
+      <c r="B38" t="s">
+        <v>260</v>
+      </c>
+      <c r="D38" t="s">
+        <v>321</v>
+      </c>
+      <c r="G38" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>262</v>
+      </c>
+      <c r="B39" t="s">
+        <v>260</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1049</v>
+      </c>
+      <c r="G39" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>9</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B40" t="s">
         <v>10</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
         <v>12</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E41" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>9</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B42" t="s">
         <v>10</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D42" t="s">
         <v>11</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E42" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>9</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B43" t="s">
         <v>10</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D43" t="s">
         <v>26</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E43" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>9</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B44" t="s">
         <v>10</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D44" t="s">
         <v>147</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E44" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>9</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B45" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D45" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E45" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>273</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B46" t="s">
         <v>276</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D46" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>273</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B47" t="s">
         <v>274</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D47" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>19</v>
-      </c>
-      <c r="B39" t="s">
-        <v>16</v>
-      </c>
-      <c r="D39" t="s">
-        <v>21</v>
-      </c>
-      <c r="E39" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>19</v>
-      </c>
-      <c r="B40" t="s">
-        <v>16</v>
-      </c>
-      <c r="D40" t="s">
-        <v>22</v>
-      </c>
-      <c r="E40" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" t="s">
-        <v>16</v>
-      </c>
-      <c r="D41" t="s">
-        <v>23</v>
-      </c>
-      <c r="E41" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" t="s">
-        <v>16</v>
-      </c>
-      <c r="D42" t="s">
-        <v>20</v>
-      </c>
-      <c r="E42" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>19</v>
-      </c>
-      <c r="B43" t="s">
-        <v>16</v>
-      </c>
-      <c r="D43" t="s">
-        <v>65</v>
-      </c>
-      <c r="E43" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>19</v>
-      </c>
-      <c r="B44" t="s">
-        <v>16</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E44" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>19</v>
-      </c>
-      <c r="B45" t="s">
-        <v>16</v>
-      </c>
-      <c r="D45" t="s">
-        <v>138</v>
-      </c>
-      <c r="E45" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>19</v>
-      </c>
-      <c r="B46" t="s">
-        <v>16</v>
-      </c>
-      <c r="D46" t="s">
-        <v>139</v>
-      </c>
-      <c r="E46" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>19</v>
-      </c>
-      <c r="B47" t="s">
-        <v>16</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="E47" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>19</v>
       </c>
@@ -4322,10 +4325,10 @@
         <v>16</v>
       </c>
       <c r="D48" t="s">
-        <v>303</v>
+        <v>21</v>
       </c>
       <c r="E48" t="s">
-        <v>191</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -4336,10 +4339,10 @@
         <v>16</v>
       </c>
       <c r="D49" t="s">
-        <v>856</v>
+        <v>22</v>
       </c>
       <c r="E49" t="s">
-        <v>809</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -4347,10 +4350,13 @@
         <v>19</v>
       </c>
       <c r="B50" t="s">
-        <v>122</v>
+        <v>16</v>
       </c>
       <c r="D50" t="s">
-        <v>187</v>
+        <v>23</v>
+      </c>
+      <c r="E50" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -4358,10 +4364,13 @@
         <v>19</v>
       </c>
       <c r="B51" t="s">
-        <v>286</v>
+        <v>16</v>
       </c>
       <c r="D51" t="s">
-        <v>298</v>
+        <v>20</v>
+      </c>
+      <c r="E51" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -4369,136 +4378,130 @@
         <v>19</v>
       </c>
       <c r="B52" t="s">
-        <v>503</v>
+        <v>16</v>
       </c>
       <c r="D52" t="s">
-        <v>504</v>
+        <v>65</v>
+      </c>
+      <c r="E52" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B53" t="s">
-        <v>30</v>
-      </c>
-      <c r="D53" t="s">
-        <v>34</v>
+        <v>16</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="E53" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B54" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D54" t="s">
-        <v>66</v>
+        <v>138</v>
       </c>
       <c r="E54" t="s">
-        <v>62</v>
+        <v>123</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B55" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D55" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="E55" t="s">
-        <v>18</v>
+        <v>125</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B56" t="s">
-        <v>30</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>217</v>
+        <v>16</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>278</v>
       </c>
       <c r="E56" t="s">
-        <v>82</v>
+        <v>279</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B57" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D57" t="s">
-        <v>218</v>
+        <v>303</v>
       </c>
       <c r="E57" t="s">
-        <v>125</v>
+        <v>191</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B58" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D58" t="s">
-        <v>220</v>
+        <v>853</v>
       </c>
       <c r="E58" t="s">
-        <v>191</v>
+        <v>806</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B59" t="s">
-        <v>30</v>
+        <v>122</v>
       </c>
       <c r="D59" t="s">
-        <v>221</v>
-      </c>
-      <c r="E59" t="s">
-        <v>123</v>
+        <v>187</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B60" t="s">
-        <v>30</v>
+        <v>286</v>
       </c>
       <c r="D60" t="s">
-        <v>254</v>
-      </c>
-      <c r="E60" t="s">
-        <v>246</v>
+        <v>298</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B61" t="s">
-        <v>30</v>
+        <v>503</v>
       </c>
       <c r="D61" t="s">
-        <v>255</v>
-      </c>
-      <c r="E61" t="s">
-        <v>2</v>
+        <v>504</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -4509,10 +4512,10 @@
         <v>30</v>
       </c>
       <c r="D62" t="s">
-        <v>857</v>
+        <v>34</v>
       </c>
       <c r="E62" t="s">
-        <v>847</v>
+        <v>24</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -4523,10 +4526,10 @@
         <v>30</v>
       </c>
       <c r="D63" t="s">
-        <v>858</v>
+        <v>66</v>
       </c>
       <c r="E63" t="s">
-        <v>809</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -4537,10 +4540,10 @@
         <v>30</v>
       </c>
       <c r="D64" t="s">
-        <v>970</v>
+        <v>67</v>
       </c>
       <c r="E64" t="s">
-        <v>966</v>
+        <v>18</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -4548,10 +4551,13 @@
         <v>32</v>
       </c>
       <c r="B65" t="s">
-        <v>7</v>
-      </c>
-      <c r="D65" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E65" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -4559,10 +4565,13 @@
         <v>32</v>
       </c>
       <c r="B66" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D66" t="s">
-        <v>42</v>
+        <v>218</v>
+      </c>
+      <c r="E66" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -4570,13 +4579,13 @@
         <v>32</v>
       </c>
       <c r="B67" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D67" t="s">
-        <v>51</v>
-      </c>
-      <c r="F67" t="s">
-        <v>3</v>
+        <v>220</v>
+      </c>
+      <c r="E67" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -4584,13 +4593,13 @@
         <v>32</v>
       </c>
       <c r="B68" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D68" t="s">
-        <v>52</v>
-      </c>
-      <c r="F68" t="s">
-        <v>24</v>
+        <v>221</v>
+      </c>
+      <c r="E68" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -4598,13 +4607,13 @@
         <v>32</v>
       </c>
       <c r="B69" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D69" t="s">
-        <v>64</v>
-      </c>
-      <c r="F69" t="s">
-        <v>62</v>
+        <v>254</v>
+      </c>
+      <c r="E69" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -4612,13 +4621,13 @@
         <v>32</v>
       </c>
       <c r="B70" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D70" t="s">
-        <v>216</v>
-      </c>
-      <c r="F70" t="s">
-        <v>18</v>
+        <v>255</v>
+      </c>
+      <c r="E70" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -4626,13 +4635,13 @@
         <v>32</v>
       </c>
       <c r="B71" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D71" t="s">
-        <v>252</v>
-      </c>
-      <c r="F71" t="s">
-        <v>125</v>
+        <v>854</v>
+      </c>
+      <c r="E71" t="s">
+        <v>844</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -4640,13 +4649,13 @@
         <v>32</v>
       </c>
       <c r="B72" t="s">
-        <v>45</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="F72" t="s">
-        <v>82</v>
+        <v>30</v>
+      </c>
+      <c r="D72" t="s">
+        <v>855</v>
+      </c>
+      <c r="E72" t="s">
+        <v>806</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -4654,13 +4663,13 @@
         <v>32</v>
       </c>
       <c r="B73" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D73" t="s">
-        <v>256</v>
-      </c>
-      <c r="F73" t="s">
-        <v>2</v>
+        <v>967</v>
+      </c>
+      <c r="E73" t="s">
+        <v>963</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -4668,13 +4677,10 @@
         <v>32</v>
       </c>
       <c r="B74" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="D74" t="s">
-        <v>272</v>
-      </c>
-      <c r="F74" t="s">
-        <v>123</v>
+        <v>27</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -4682,13 +4688,10 @@
         <v>32</v>
       </c>
       <c r="B75" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D75" t="s">
-        <v>301</v>
-      </c>
-      <c r="F75" t="s">
-        <v>191</v>
+        <v>42</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -4699,10 +4702,10 @@
         <v>45</v>
       </c>
       <c r="D76" t="s">
-        <v>859</v>
+        <v>51</v>
       </c>
       <c r="F76" t="s">
-        <v>809</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -4710,10 +4713,13 @@
         <v>32</v>
       </c>
       <c r="B77" t="s">
-        <v>260</v>
+        <v>45</v>
       </c>
       <c r="D77" t="s">
-        <v>267</v>
+        <v>52</v>
+      </c>
+      <c r="F77" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -4721,10 +4727,13 @@
         <v>32</v>
       </c>
       <c r="B78" t="s">
-        <v>286</v>
+        <v>45</v>
       </c>
       <c r="D78" t="s">
-        <v>298</v>
+        <v>64</v>
+      </c>
+      <c r="F78" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -4732,20 +4741,140 @@
         <v>32</v>
       </c>
       <c r="B79" t="s">
-        <v>503</v>
+        <v>45</v>
       </c>
       <c r="D79" t="s">
-        <v>504</v>
+        <v>216</v>
+      </c>
+      <c r="F79" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>32</v>
+      </c>
+      <c r="B80" t="s">
+        <v>45</v>
+      </c>
+      <c r="D80" t="s">
+        <v>252</v>
+      </c>
+      <c r="F80" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>32</v>
+      </c>
+      <c r="B81" t="s">
+        <v>45</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="F81" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>32</v>
+      </c>
+      <c r="B82" t="s">
+        <v>45</v>
+      </c>
+      <c r="D82" t="s">
+        <v>256</v>
+      </c>
+      <c r="F82" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>32</v>
+      </c>
+      <c r="B83" t="s">
+        <v>45</v>
+      </c>
+      <c r="D83" t="s">
+        <v>272</v>
+      </c>
+      <c r="F83" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>32</v>
+      </c>
+      <c r="B84" t="s">
+        <v>45</v>
+      </c>
+      <c r="D84" t="s">
+        <v>301</v>
+      </c>
+      <c r="F84" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>32</v>
+      </c>
+      <c r="B85" t="s">
+        <v>45</v>
+      </c>
+      <c r="D85" t="s">
+        <v>856</v>
+      </c>
+      <c r="F85" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>32</v>
+      </c>
+      <c r="B86" t="s">
+        <v>260</v>
+      </c>
+      <c r="D86" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>32</v>
+      </c>
+      <c r="B87" t="s">
+        <v>286</v>
+      </c>
+      <c r="D87" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>32</v>
+      </c>
+      <c r="B88" t="s">
+        <v>503</v>
+      </c>
+      <c r="D88" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>133</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B89" t="s">
         <v>269</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D89" t="s">
         <v>270</v>
       </c>
     </row>
@@ -5191,13 +5320,13 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="C27" t="s">
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="E27" t="s">
         <v>140</v>
@@ -5589,7 +5718,7 @@
         <v>287</v>
       </c>
       <c r="G6" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -6043,16 +6172,16 @@
         <v>143</v>
       </c>
       <c r="B29" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="C29" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="D29" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="E29" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="F29" t="s">
         <v>290</v>
@@ -6063,16 +6192,16 @@
         <v>143</v>
       </c>
       <c r="B30" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="C30" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="D30" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="E30" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="F30" t="s">
         <v>290</v>
@@ -6083,16 +6212,16 @@
         <v>143</v>
       </c>
       <c r="B31" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="C31" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="D31" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="E31" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="F31" t="s">
         <v>290</v>
@@ -6103,16 +6232,16 @@
         <v>143</v>
       </c>
       <c r="B32" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
       <c r="C32" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="D32" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="E32" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="F32" t="s">
         <v>290</v>
@@ -6123,16 +6252,16 @@
         <v>143</v>
       </c>
       <c r="B33" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="C33" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="D33" t="s">
         <v>336</v>
       </c>
       <c r="E33" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
       <c r="F33" t="s">
         <v>290</v>
@@ -6147,8 +6276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6208,7 +6337,7 @@
         <v>503</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -6249,7 +6378,7 @@
         <v>505</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -6371,7 +6500,7 @@
         <v>509</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -6412,7 +6541,7 @@
         <v>510</v>
       </c>
       <c r="N6" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -6453,7 +6582,7 @@
         <v>511</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -6488,7 +6617,7 @@
         <v>289</v>
       </c>
       <c r="M8" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
       <c r="N8" s="4"/>
     </row>
@@ -6530,7 +6659,7 @@
         <v>514</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -6547,10 +6676,10 @@
         <v>159</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>3</v>
@@ -6571,7 +6700,7 @@
         <v>514</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -6609,7 +6738,7 @@
         <v>511</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -6620,19 +6749,19 @@
         <v>17</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>336</v>
@@ -6647,7 +6776,7 @@
         <v>511</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -6688,7 +6817,7 @@
         <v>514</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -6708,7 +6837,7 @@
         <v>24</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>2</v>
@@ -6729,7 +6858,7 @@
         <v>514</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -6764,10 +6893,10 @@
         <v>289</v>
       </c>
       <c r="M15" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -6808,7 +6937,7 @@
         <v>513</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -6819,7 +6948,7 @@
         <v>669</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>169</v>
@@ -6847,7 +6976,7 @@
         <v>621</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -6923,7 +7052,7 @@
         <v>628</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -6955,7 +7084,7 @@
         <v>72</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="L20" s="4" t="s">
         <v>290</v>
@@ -6964,7 +7093,7 @@
         <v>647</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -6975,10 +7104,10 @@
         <v>17</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>24</v>
@@ -6996,16 +7125,16 @@
         <v>72</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="L21" s="4" t="s">
         <v>290</v>
       </c>
       <c r="M21" s="11" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -7016,10 +7145,10 @@
         <v>17</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>1035</v>
+        <v>1032</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>24</v>
@@ -7041,10 +7170,10 @@
         <v>290</v>
       </c>
       <c r="M22" s="11" t="s">
-        <v>1041</v>
+        <v>1038</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>1047</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -7079,10 +7208,10 @@
         <v>289</v>
       </c>
       <c r="M23" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -7123,7 +7252,7 @@
         <v>648</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>1046</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -7161,7 +7290,7 @@
         <v>649</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -7202,7 +7331,7 @@
         <v>652</v>
       </c>
       <c r="N26" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -7243,7 +7372,7 @@
         <v>668</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -7254,16 +7383,16 @@
         <v>17</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="D28" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>2</v>
@@ -7275,13 +7404,13 @@
         <v>71</v>
       </c>
       <c r="K28" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="L28" s="4" t="s">
         <v>287</v>
       </c>
       <c r="M28" s="11" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="N28" s="4"/>
     </row>
@@ -7293,22 +7422,22 @@
         <v>17</v>
       </c>
       <c r="C29" s="9" t="s">
+        <v>804</v>
+      </c>
+      <c r="D29" t="s">
+        <v>805</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>806</v>
+      </c>
+      <c r="F29" s="9" t="s">
         <v>807</v>
       </c>
-      <c r="D29" t="s">
+      <c r="G29" s="4" t="s">
+        <v>806</v>
+      </c>
+      <c r="H29" s="9" t="s">
         <v>808</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>809</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>810</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>809</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>811</v>
       </c>
       <c r="J29" s="8" t="s">
         <v>72</v>
@@ -7320,7 +7449,7 @@
         <v>647</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -7331,10 +7460,10 @@
         <v>17</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="D30" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>24</v>
@@ -7358,10 +7487,10 @@
         <v>289</v>
       </c>
       <c r="M30" s="11" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="N30" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="60" x14ac:dyDescent="0.25">
@@ -7372,16 +7501,16 @@
         <v>17</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
       <c r="D31" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>3</v>
@@ -7399,10 +7528,10 @@
         <v>289</v>
       </c>
       <c r="M31" s="21" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -7413,16 +7542,16 @@
         <v>17</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>82</v>
@@ -7440,7 +7569,7 @@
         <v>511</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -7451,16 +7580,16 @@
         <v>17</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>1011</v>
+        <v>1008</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>82</v>
@@ -7478,7 +7607,7 @@
         <v>511</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -7510,16 +7639,16 @@
         <v>73</v>
       </c>
       <c r="K34" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="L34" s="4" t="s">
         <v>287</v>
       </c>
       <c r="M34" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="N34" s="4" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -7554,10 +7683,10 @@
         <v>289</v>
       </c>
       <c r="M35" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="N35" s="4" t="s">
-        <v>989</v>
+        <v>986</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -7595,10 +7724,10 @@
         <v>290</v>
       </c>
       <c r="M36" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="N36" s="4" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -7633,10 +7762,10 @@
         <v>289</v>
       </c>
       <c r="M37" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="N37" s="4" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -7671,10 +7800,10 @@
         <v>289</v>
       </c>
       <c r="M38" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="N38" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -7712,10 +7841,10 @@
         <v>290</v>
       </c>
       <c r="M39" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="N39" t="s">
-        <v>1045</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -7726,16 +7855,16 @@
         <v>77</v>
       </c>
       <c r="C40" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
       <c r="D40" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="F40" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>3</v>
@@ -7753,10 +7882,10 @@
         <v>290</v>
       </c>
       <c r="M40" s="11" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
@@ -7767,16 +7896,16 @@
         <v>77</v>
       </c>
       <c r="C41" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
       <c r="D41" t="s">
-        <v>974</v>
+        <v>971</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>125</v>
       </c>
       <c r="F41" t="s">
-        <v>975</v>
+        <v>972</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>2</v>
@@ -7789,10 +7918,10 @@
         <v>290</v>
       </c>
       <c r="M41" s="11" t="s">
-        <v>976</v>
+        <v>973</v>
       </c>
       <c r="N41" s="4" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -7830,7 +7959,7 @@
         <v>513</v>
       </c>
       <c r="N42" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
@@ -7868,7 +7997,7 @@
         <v>287</v>
       </c>
       <c r="M43" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -7903,10 +8032,10 @@
         <v>290</v>
       </c>
       <c r="M44" s="3" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="N44" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -7944,7 +8073,7 @@
         <v>287</v>
       </c>
       <c r="M45" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -7958,7 +8087,7 @@
         <v>43</v>
       </c>
       <c r="D46" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>24</v>
@@ -7979,10 +8108,10 @@
         <v>290</v>
       </c>
       <c r="M46" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="N46" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
@@ -8020,7 +8149,7 @@
         <v>287</v>
       </c>
       <c r="M47" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
@@ -8031,16 +8160,16 @@
         <v>78</v>
       </c>
       <c r="C48" s="4" t="s">
+        <v>961</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>962</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>963</v>
+      </c>
+      <c r="F48" s="4" t="s">
         <v>964</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>965</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>966</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>967</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>3</v>
@@ -8058,10 +8187,10 @@
         <v>290</v>
       </c>
       <c r="M48" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
       <c r="N48" s="4" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
@@ -8411,10 +8540,10 @@
         <v>289</v>
       </c>
       <c r="M58" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="N58" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
@@ -8828,7 +8957,7 @@
         <v>621</v>
       </c>
       <c r="N70" t="s">
-        <v>997</v>
+        <v>994</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
@@ -8866,7 +8995,7 @@
         <v>649</v>
       </c>
       <c r="N71" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
@@ -8877,16 +9006,16 @@
         <v>63</v>
       </c>
       <c r="C72" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="D72" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="E72" t="s">
         <v>62</v>
       </c>
       <c r="F72" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>3</v>
@@ -8915,7 +9044,7 @@
         <v>63</v>
       </c>
       <c r="C73" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="D73" t="s">
         <v>228</v>
@@ -8924,7 +9053,7 @@
         <v>62</v>
       </c>
       <c r="F73" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="G73" s="4" t="s">
         <v>3</v>
@@ -8980,7 +9109,7 @@
         <v>287</v>
       </c>
       <c r="M74" s="3" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
     </row>
     <row r="75" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9018,7 +9147,7 @@
         <v>287</v>
       </c>
       <c r="M75" s="3" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
     </row>
     <row r="76" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9029,10 +9158,10 @@
         <v>130</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="D76" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="E76" t="s">
         <v>24</v>
@@ -9056,7 +9185,7 @@
         <v>289</v>
       </c>
       <c r="M76" s="3" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
     </row>
     <row r="77" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9091,10 +9220,10 @@
         <v>290</v>
       </c>
       <c r="M77" s="11" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="N77" t="s">
-        <v>1040</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
@@ -9102,25 +9231,25 @@
         <v>905</v>
       </c>
       <c r="B78" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="C78" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="D78" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="E78" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="F78" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="H78" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="J78" t="s">
         <v>73</v>
@@ -9129,7 +9258,7 @@
         <v>287</v>
       </c>
       <c r="M78" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
@@ -9137,13 +9266,13 @@
         <v>906</v>
       </c>
       <c r="B79" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="C79" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="D79" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="E79" t="s">
         <v>24</v>
@@ -9161,13 +9290,13 @@
         <v>73</v>
       </c>
       <c r="K79" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="L79" t="s">
         <v>287</v>
       </c>
       <c r="M79" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.25">
@@ -9175,13 +9304,13 @@
         <v>907</v>
       </c>
       <c r="B80" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="C80" t="s">
         <v>31</v>
       </c>
       <c r="D80" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="E80" t="s">
         <v>24</v>
@@ -9205,7 +9334,7 @@
         <v>290</v>
       </c>
       <c r="M80" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
@@ -9213,25 +9342,25 @@
         <v>908</v>
       </c>
       <c r="B81" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="C81" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="D81" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="E81" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="F81" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="H81" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="J81" t="s">
         <v>73</v>
@@ -9240,7 +9369,7 @@
         <v>287</v>
       </c>
       <c r="M81" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
@@ -9248,25 +9377,25 @@
         <v>909</v>
       </c>
       <c r="B82" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="C82" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="D82" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="E82" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="F82" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="H82" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="J82" t="s">
         <v>73</v>
@@ -9275,7 +9404,7 @@
         <v>287</v>
       </c>
       <c r="M82" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
@@ -9283,19 +9412,19 @@
         <v>910</v>
       </c>
       <c r="B83" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
       <c r="C83" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="D83" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="E83" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="F83" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="G83" s="4" t="s">
         <v>24</v>
@@ -9310,7 +9439,7 @@
         <v>287</v>
       </c>
       <c r="M83" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
@@ -9318,13 +9447,13 @@
         <v>911</v>
       </c>
       <c r="B84" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="C84" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="D84" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="E84" t="s">
         <v>24</v>
@@ -9342,13 +9471,13 @@
         <v>73</v>
       </c>
       <c r="K84" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="L84" t="s">
         <v>287</v>
       </c>
       <c r="M84" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
@@ -9356,19 +9485,19 @@
         <v>912</v>
       </c>
       <c r="B85" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="C85" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="D85" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
       <c r="E85" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="F85" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
       <c r="G85" s="4" t="s">
         <v>62</v>
@@ -9383,7 +9512,7 @@
         <v>287</v>
       </c>
       <c r="M85" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
     </row>
   </sheetData>
@@ -9515,10 +9644,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="B13" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="C13" t="s">
         <v>658</v>
@@ -9526,21 +9655,21 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="B14" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="C14" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>963</v>
+      </c>
+      <c r="B15" t="s">
         <v>966</v>
-      </c>
-      <c r="B15" t="s">
-        <v>969</v>
       </c>
     </row>
   </sheetData>
@@ -9604,8 +9733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9623,7 +9752,7 @@
         <v>260</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>328</v>
@@ -9649,16 +9778,16 @@
         <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="C2" t="s">
         <v>334</v>
       </c>
       <c r="D2" t="s">
+        <v>676</v>
+      </c>
+      <c r="E2" t="s">
         <v>677</v>
-      </c>
-      <c r="E2" t="s">
-        <v>678</v>
       </c>
       <c r="G2" t="s">
         <v>445</v>
@@ -9672,16 +9801,16 @@
         <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C3" t="s">
         <v>334</v>
       </c>
       <c r="D3" t="s">
-        <v>682</v>
+        <v>676</v>
       </c>
       <c r="E3" t="s">
-        <v>683</v>
+        <v>677</v>
       </c>
       <c r="G3" t="s">
         <v>445</v>
@@ -9690,7 +9819,7 @@
         <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -9698,7 +9827,7 @@
         <v>304</v>
       </c>
       <c r="B4" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C4" t="s">
         <v>329</v>
@@ -9721,16 +9850,16 @@
         <v>304</v>
       </c>
       <c r="B5" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="C5" t="s">
         <v>329</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>909</v>
+        <v>906</v>
       </c>
       <c r="E5" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="G5" t="s">
         <v>444</v>
@@ -9847,7 +9976,7 @@
         <v>315</v>
       </c>
       <c r="B11" t="s">
-        <v>671</v>
+        <v>675</v>
       </c>
       <c r="C11" t="s">
         <v>332</v>
@@ -9870,7 +9999,7 @@
         <v>315</v>
       </c>
       <c r="B12" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C12" t="s">
         <v>332</v>
@@ -9893,13 +10022,16 @@
         <v>315</v>
       </c>
       <c r="B13" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C13" t="s">
         <v>332</v>
       </c>
       <c r="D13" t="s">
         <v>322</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1049</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -9930,10 +10062,10 @@
         <v>329</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="E15" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="G15" t="s">
         <v>444</v>
@@ -9950,10 +10082,10 @@
         <v>329</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="E16" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="G16" t="s">
         <v>444</v>
@@ -9964,16 +10096,16 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="C17" t="s">
         <v>329</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="E17" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="G17" t="s">
         <v>444</v>
@@ -9984,16 +10116,16 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="C18" t="s">
         <v>329</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="E18" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="G18" t="s">
         <v>444</v>
@@ -10004,16 +10136,16 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="C19" t="s">
         <v>329</v>
       </c>
       <c r="D19" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
       <c r="E19" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="G19" t="s">
         <v>444</v>
@@ -10024,16 +10156,16 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="C20" t="s">
         <v>329</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
       <c r="E20" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
       <c r="G20" t="s">
         <v>444</v>
@@ -10044,16 +10176,16 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
       <c r="C21" t="s">
         <v>329</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
       <c r="E21" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
       <c r="G21" t="s">
         <v>444</v>
@@ -10064,13 +10196,13 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="C22" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="G22" t="s">
         <v>444</v>
@@ -10081,16 +10213,16 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="C23" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
       <c r="E23" t="s">
-        <v>1025</v>
+        <v>1022</v>
       </c>
       <c r="G23" t="s">
         <v>445</v>
@@ -10098,16 +10230,16 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
       <c r="C24" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="E24" t="s">
-        <v>1039</v>
+        <v>1036</v>
       </c>
       <c r="G24" t="s">
         <v>445</v>
@@ -10116,7 +10248,7 @@
         <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>1043</v>
+        <v>1040</v>
       </c>
     </row>
   </sheetData>
@@ -10129,8 +10261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E176"/>
   <sheetViews>
-    <sheetView topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="A176" sqref="A176"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58:A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10147,7 +10279,7 @@
         <v>260</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>261</v>
@@ -11085,13 +11217,13 @@
         <v>306</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
       <c r="D56" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
       <c r="E56" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -11102,13 +11234,13 @@
         <v>306</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>911</v>
+        <v>908</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -11116,7 +11248,7 @@
         <v>315</v>
       </c>
       <c r="B58" t="s">
-        <v>315</v>
+        <v>670</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>493</v>
@@ -11133,7 +11265,7 @@
         <v>315</v>
       </c>
       <c r="B59" t="s">
-        <v>315</v>
+        <v>675</v>
       </c>
       <c r="C59" t="s">
         <v>485</v>
@@ -11150,7 +11282,7 @@
         <v>315</v>
       </c>
       <c r="B60" t="s">
-        <v>315</v>
+        <v>675</v>
       </c>
       <c r="C60" t="s">
         <v>488</v>
@@ -11167,7 +11299,7 @@
         <v>315</v>
       </c>
       <c r="B61" t="s">
-        <v>315</v>
+        <v>675</v>
       </c>
       <c r="C61" t="s">
         <v>476</v>
@@ -11184,7 +11316,7 @@
         <v>315</v>
       </c>
       <c r="B62" t="s">
-        <v>315</v>
+        <v>671</v>
       </c>
       <c r="C62" t="s">
         <v>494</v>
@@ -11201,7 +11333,7 @@
         <v>315</v>
       </c>
       <c r="B63" t="s">
-        <v>315</v>
+        <v>671</v>
       </c>
       <c r="C63" t="s">
         <v>497</v>
@@ -11218,7 +11350,7 @@
         <v>315</v>
       </c>
       <c r="B64" t="s">
-        <v>315</v>
+        <v>671</v>
       </c>
       <c r="C64" t="s">
         <v>499</v>
@@ -11235,7 +11367,7 @@
         <v>304</v>
       </c>
       <c r="B65" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C65" t="s">
         <v>517</v>
@@ -11252,7 +11384,7 @@
         <v>304</v>
       </c>
       <c r="B66" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C66" t="s">
         <v>520</v>
@@ -11269,7 +11401,7 @@
         <v>304</v>
       </c>
       <c r="B67" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C67" t="s">
         <v>523</v>
@@ -11286,7 +11418,7 @@
         <v>304</v>
       </c>
       <c r="B68" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C68" t="s">
         <v>526</v>
@@ -11303,7 +11435,7 @@
         <v>304</v>
       </c>
       <c r="B69" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C69" t="s">
         <v>529</v>
@@ -11320,7 +11452,7 @@
         <v>304</v>
       </c>
       <c r="B70" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C70" t="s">
         <v>532</v>
@@ -11337,7 +11469,7 @@
         <v>304</v>
       </c>
       <c r="B71" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C71" t="s">
         <v>535</v>
@@ -11354,7 +11486,7 @@
         <v>304</v>
       </c>
       <c r="B72" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C72" t="s">
         <v>538</v>
@@ -11371,7 +11503,7 @@
         <v>304</v>
       </c>
       <c r="B73" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C73" t="s">
         <v>541</v>
@@ -11388,7 +11520,7 @@
         <v>304</v>
       </c>
       <c r="B74" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C74" t="s">
         <v>544</v>
@@ -11405,7 +11537,7 @@
         <v>304</v>
       </c>
       <c r="B75" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C75" t="s">
         <v>547</v>
@@ -11422,7 +11554,7 @@
         <v>304</v>
       </c>
       <c r="B76" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C76" t="s">
         <v>550</v>
@@ -11439,7 +11571,7 @@
         <v>304</v>
       </c>
       <c r="B77" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C77" t="s">
         <v>553</v>
@@ -11456,7 +11588,7 @@
         <v>304</v>
       </c>
       <c r="B78" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C78" t="s">
         <v>556</v>
@@ -11473,7 +11605,7 @@
         <v>304</v>
       </c>
       <c r="B79" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C79" t="s">
         <v>559</v>
@@ -11490,7 +11622,7 @@
         <v>304</v>
       </c>
       <c r="B80" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C80" t="s">
         <v>562</v>
@@ -11507,7 +11639,7 @@
         <v>304</v>
       </c>
       <c r="B81" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C81" t="s">
         <v>565</v>
@@ -11524,7 +11656,7 @@
         <v>304</v>
       </c>
       <c r="B82" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C82" t="s">
         <v>568</v>
@@ -11541,7 +11673,7 @@
         <v>304</v>
       </c>
       <c r="B83" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C83" t="s">
         <v>571</v>
@@ -11558,7 +11690,7 @@
         <v>304</v>
       </c>
       <c r="B84" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C84" t="s">
         <v>574</v>
@@ -11575,7 +11707,7 @@
         <v>304</v>
       </c>
       <c r="B85" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C85" t="s">
         <v>577</v>
@@ -11592,7 +11724,7 @@
         <v>304</v>
       </c>
       <c r="B86" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C86" t="s">
         <v>580</v>
@@ -11609,7 +11741,7 @@
         <v>304</v>
       </c>
       <c r="B87" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C87" t="s">
         <v>583</v>
@@ -11626,7 +11758,7 @@
         <v>304</v>
       </c>
       <c r="B88" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C88" t="s">
         <v>586</v>
@@ -11643,7 +11775,7 @@
         <v>304</v>
       </c>
       <c r="B89" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C89" t="s">
         <v>589</v>
@@ -11660,7 +11792,7 @@
         <v>304</v>
       </c>
       <c r="B90" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C90" t="s">
         <v>592</v>
@@ -11677,7 +11809,7 @@
         <v>304</v>
       </c>
       <c r="B91" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C91" t="s">
         <v>595</v>
@@ -11694,7 +11826,7 @@
         <v>304</v>
       </c>
       <c r="B92" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C92" t="s">
         <v>598</v>
@@ -11711,7 +11843,7 @@
         <v>304</v>
       </c>
       <c r="B93" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C93" t="s">
         <v>601</v>
@@ -11728,7 +11860,7 @@
         <v>304</v>
       </c>
       <c r="B94" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C94" t="s">
         <v>604</v>
@@ -11745,7 +11877,7 @@
         <v>304</v>
       </c>
       <c r="B95" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C95" t="s">
         <v>607</v>
@@ -11762,7 +11894,7 @@
         <v>304</v>
       </c>
       <c r="B96" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C96" t="s">
         <v>610</v>
@@ -11779,7 +11911,7 @@
         <v>304</v>
       </c>
       <c r="B97" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C97" t="s">
         <v>613</v>
@@ -11796,7 +11928,7 @@
         <v>304</v>
       </c>
       <c r="B98" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C98" t="s">
         <v>616</v>
@@ -11813,7 +11945,7 @@
         <v>304</v>
       </c>
       <c r="B99" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="C99" t="s">
         <v>619</v>
@@ -11830,16 +11962,16 @@
         <v>304</v>
       </c>
       <c r="B100" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="C100" s="20" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
       <c r="D100" s="20" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
       <c r="E100" s="20" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -11847,16 +11979,16 @@
         <v>304</v>
       </c>
       <c r="B101" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="C101" s="20" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="D101" s="20" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="E101" s="20" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -11864,16 +11996,16 @@
         <v>304</v>
       </c>
       <c r="B102" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="C102" s="20" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
       <c r="D102" s="20" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
       <c r="E102" s="20" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -11881,16 +12013,16 @@
         <v>304</v>
       </c>
       <c r="B103" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="C103" s="20" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
       <c r="D103" s="20" t="s">
-        <v>926</v>
+        <v>923</v>
       </c>
       <c r="E103" s="20" t="s">
-        <v>927</v>
+        <v>924</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -11898,16 +12030,16 @@
         <v>304</v>
       </c>
       <c r="B104" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="C104" s="20" t="s">
-        <v>928</v>
+        <v>925</v>
       </c>
       <c r="D104" s="20" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="E104" s="20" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -11915,16 +12047,16 @@
         <v>304</v>
       </c>
       <c r="B105" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="C105" s="20" t="s">
-        <v>929</v>
+        <v>926</v>
       </c>
       <c r="D105" s="20" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="E105" s="20" t="s">
-        <v>931</v>
+        <v>928</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -11932,16 +12064,16 @@
         <v>304</v>
       </c>
       <c r="B106" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="C106" s="20" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
       <c r="D106" s="20" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="E106" s="20" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -11949,16 +12081,16 @@
         <v>304</v>
       </c>
       <c r="B107" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="C107" s="20" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
       <c r="D107" s="20" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
       <c r="E107" s="20" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -11966,16 +12098,16 @@
         <v>304</v>
       </c>
       <c r="B108" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="C108" s="20" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
       <c r="D108" s="20" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
       <c r="E108" s="20" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -11983,7 +12115,7 @@
         <v>304</v>
       </c>
       <c r="B109" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="C109" s="20" t="s">
         <v>440</v>
@@ -12000,16 +12132,16 @@
         <v>304</v>
       </c>
       <c r="B110" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="C110" s="20" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
       <c r="D110" s="20" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
       <c r="E110" s="20" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -12017,16 +12149,16 @@
         <v>304</v>
       </c>
       <c r="B111" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="C111" s="20" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
       <c r="D111" s="20" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
       <c r="E111" s="20" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -12034,16 +12166,16 @@
         <v>304</v>
       </c>
       <c r="B112" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="C112" s="20" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="D112" s="20" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="E112" s="20" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -12051,16 +12183,16 @@
         <v>304</v>
       </c>
       <c r="B113" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="C113" s="20" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
       <c r="D113" s="20" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
       <c r="E113" s="20" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -12245,13 +12377,13 @@
         <v>111</v>
       </c>
       <c r="B126" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -12259,13 +12391,13 @@
         <v>111</v>
       </c>
       <c r="B127" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C127" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="D127" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -12273,13 +12405,13 @@
         <v>111</v>
       </c>
       <c r="B128" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C128" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="D128" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -12287,296 +12419,296 @@
         <v>111</v>
       </c>
       <c r="B129" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C129" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="D129" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="B130" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="C130" s="19" t="s">
         <v>408</v>
       </c>
       <c r="D130" s="19" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="E130" s="19" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="B131" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="C131" s="19" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="D131" s="19" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="E131" s="19" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="B132" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="C132" s="19" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="D132" s="19" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="E132" s="19" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="B133" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="C133" s="19" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="D133" s="19" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="E133" s="19" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="B134" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="C134" s="19" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="D134" s="19" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="E134" s="19" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="B135" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="C135" s="19" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="D135" s="19" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="E135" s="19" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
+        <v>746</v>
+      </c>
+      <c r="B136" t="s">
+        <v>746</v>
+      </c>
+      <c r="C136" s="20" t="s">
         <v>749</v>
       </c>
-      <c r="B136" t="s">
-        <v>749</v>
-      </c>
-      <c r="C136" s="20" t="s">
-        <v>752</v>
-      </c>
       <c r="D136" s="20" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="E136" s="20" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="B137" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="C137" s="20" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="D137" s="20" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="E137" s="20" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="B138" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="C138" s="20" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="D138" s="20" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="E138" s="20" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="B139" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="C139" s="20" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="D139" s="20" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="E139" s="20" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="B140" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="C140" s="20" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="D140" s="20" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="E140" s="20" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="B141" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="C141" s="20" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="D141" s="20" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="E141" s="20" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="B142" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="C142" s="20" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="D142" s="20" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="E142" s="20" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="B143" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="C143" s="20" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="D143" s="20" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="E143" s="20" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="B144" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="C144" s="20" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="D144" s="20" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="E144" s="20" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="B145" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="C145" s="20" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="D145" s="20" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="E145" s="20" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="B146" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="C146" s="20" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="D146" s="20" t="s">
         <v>108</v>
@@ -12587,13 +12719,13 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="B147" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="C147" s="20" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="D147" s="20" t="s">
         <v>545</v>
@@ -12604,471 +12736,471 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="B148" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="C148" s="20" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="D148" s="20" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="E148" s="20" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="B149" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="C149" s="20" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="D149" s="20" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="E149" s="20" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="B150" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="C150" s="20" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="D150" s="20" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="E150" s="20" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="B151" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="C151" s="20" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="D151" s="20" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="E151" s="20" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="B152" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="C152" s="20" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="D152" s="20" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="E152" s="20" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="B153" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="C153" s="20" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="D153" s="20" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="E153" s="20" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="B154" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="C154" s="20" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="D154" s="20" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="E154" s="20" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="B155" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="C155" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
       <c r="D155" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="E155" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="B156" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="C156" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
       <c r="D156" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
       <c r="E156" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="B157" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="C157" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
       <c r="D157" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
       <c r="E157" t="s">
-        <v>879</v>
+        <v>876</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="B158" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="C158" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
       <c r="D158" t="s">
-        <v>881</v>
+        <v>878</v>
       </c>
       <c r="E158" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="B159" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="C159" t="s">
-        <v>883</v>
+        <v>880</v>
       </c>
       <c r="D159" t="s">
-        <v>884</v>
+        <v>881</v>
       </c>
       <c r="E159" t="s">
-        <v>885</v>
+        <v>882</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="B160" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="C160" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
       <c r="D160" t="s">
-        <v>887</v>
+        <v>884</v>
       </c>
       <c r="E160" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="B161" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="C161" t="s">
         <v>160</v>
       </c>
       <c r="D161" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
       <c r="E161" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="B162" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="C162" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
       <c r="D162" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
       <c r="E162" t="s">
-        <v>893</v>
+        <v>890</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="B163" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="C163" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
       <c r="D163" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="E163" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="B164" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="C164" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="D164" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
       <c r="E164" t="s">
-        <v>899</v>
+        <v>896</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="B165" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="C165" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="D165" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
       <c r="E165" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="B166" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="C166" s="22" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
       <c r="D166" s="22" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
       <c r="E166" s="22" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="B167" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="C167" s="22" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
       <c r="D167" s="22" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
       <c r="E167" s="22" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="B168" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="C168" s="22" t="s">
-        <v>958</v>
+        <v>955</v>
       </c>
       <c r="D168" s="22" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
       <c r="E168" s="22" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
+        <v>974</v>
+      </c>
+      <c r="B169" t="s">
+        <v>974</v>
+      </c>
+      <c r="C169" s="4" t="s">
         <v>977</v>
       </c>
-      <c r="B169" t="s">
-        <v>977</v>
-      </c>
-      <c r="C169" s="4" t="s">
+      <c r="D169" t="s">
         <v>980</v>
-      </c>
-      <c r="D169" t="s">
-        <v>983</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
       <c r="B170" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
       <c r="C170" s="4" t="s">
+        <v>978</v>
+      </c>
+      <c r="D170" t="s">
         <v>981</v>
-      </c>
-      <c r="D170" t="s">
-        <v>984</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
       <c r="B171" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
       <c r="C171" s="4" t="s">
+        <v>979</v>
+      </c>
+      <c r="D171" t="s">
         <v>982</v>
-      </c>
-      <c r="D171" t="s">
-        <v>985</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="B172" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>1022</v>
+        <v>1019</v>
       </c>
       <c r="D172" t="s">
-        <v>1023</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="B173" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="C173" s="23" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
       <c r="D173" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="B174" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="C174" s="23" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
       <c r="D174" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="B175" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="C175" s="23" t="s">
-        <v>1031</v>
+        <v>1028</v>
       </c>
       <c r="D175" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
       <c r="B176" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
       <c r="C176" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
       <c r="D176" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
     </row>
   </sheetData>

</xml_diff>